<commit_message>
Optional tag added for paramters in base class
</commit_message>
<xml_diff>
--- a/Testdata/CoursesDetails.xlsx
+++ b/Testdata/CoursesDetails.xlsx
@@ -24,28 +24,28 @@
 </t>
   </si>
   <si>
-    <t>(5,465)</t>
+    <t>(5,484)</t>
   </si>
   <si>
     <t xml:space="preserve">Intermediate
 </t>
   </si>
   <si>
-    <t>(3,501)</t>
+    <t>(3,558)</t>
   </si>
   <si>
     <t xml:space="preserve">Advanced
 </t>
   </si>
   <si>
-    <t>(378)</t>
+    <t>(383)</t>
   </si>
   <si>
     <t xml:space="preserve">Mixed
 </t>
   </si>
   <si>
-    <t>(997)</t>
+    <t>(992)</t>
   </si>
   <si>
     <t>Languages</t>
@@ -55,7 +55,7 @@
 </t>
   </si>
   <si>
-    <t>(9,140)</t>
+    <t>(9,233)</t>
   </si>
   <si>
     <t xml:space="preserve">Spanish
@@ -69,7 +69,7 @@
 </t>
   </si>
   <si>
-    <t>(4,121)</t>
+    <t>(4,130)</t>
   </si>
   <si>
     <t xml:space="preserve">French
@@ -83,175 +83,175 @@
 </t>
   </si>
   <si>
-    <t>(3,823)</t>
+    <t>(3,828)</t>
   </si>
   <si>
     <t xml:space="preserve">German
 </t>
   </si>
   <si>
-    <t>(3,778)</t>
+    <t>(3,783)</t>
   </si>
   <si>
     <t xml:space="preserve">Portuguese
 </t>
   </si>
   <si>
-    <t>(2,991)</t>
+    <t>(2,990)</t>
   </si>
   <si>
     <t xml:space="preserve">Indonesian
 </t>
   </si>
   <si>
-    <t>(2,820)</t>
+    <t>(2,823)</t>
   </si>
   <si>
     <t xml:space="preserve">Chinese
 </t>
   </si>
   <si>
-    <t>(2,649)</t>
+    <t>(2,652)</t>
   </si>
   <si>
     <t xml:space="preserve">Japanese
 </t>
   </si>
   <si>
-    <t>(2,530)</t>
+    <t>(2,533)</t>
   </si>
   <si>
     <t xml:space="preserve">Russian
 </t>
   </si>
   <si>
-    <t>(2,511)</t>
+    <t>(2,516)</t>
   </si>
   <si>
     <t xml:space="preserve">Korean
 </t>
   </si>
   <si>
-    <t>(2,478)</t>
+    <t>(2,484)</t>
   </si>
   <si>
     <t xml:space="preserve">Hindi
 </t>
   </si>
   <si>
-    <t>(2,412)</t>
+    <t>(2,417)</t>
   </si>
   <si>
     <t xml:space="preserve">Italian
 </t>
   </si>
   <si>
-    <t>(2,396)</t>
+    <t>(2,401)</t>
   </si>
   <si>
     <t xml:space="preserve">Turkish
 </t>
   </si>
   <si>
-    <t>(2,344)</t>
+    <t>(2,349)</t>
   </si>
   <si>
     <t xml:space="preserve">Thai
 </t>
   </si>
   <si>
-    <t>(2,324)</t>
+    <t>(2,328)</t>
   </si>
   <si>
     <t xml:space="preserve">Ukrainian
 </t>
   </si>
   <si>
-    <t>(2,321)</t>
+    <t>(2,325)</t>
   </si>
   <si>
     <t xml:space="preserve">Greek
 </t>
   </si>
   <si>
-    <t>(2,302)</t>
+    <t>(2,307)</t>
   </si>
   <si>
     <t xml:space="preserve">Polish
 </t>
   </si>
   <si>
+    <t>(2,288)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dutch
+</t>
+  </si>
+  <si>
     <t>(2,283)</t>
   </si>
   <si>
-    <t xml:space="preserve">Dutch
-</t>
-  </si>
-  <si>
-    <t>(2,278)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Swedish
 </t>
   </si>
   <si>
-    <t>(2,256)</t>
+    <t>(2,261)</t>
   </si>
   <si>
     <t xml:space="preserve">Hungarian
 </t>
   </si>
   <si>
-    <t>(1,923)</t>
+    <t>(1,927)</t>
   </si>
   <si>
     <t xml:space="preserve">Vietnamese
 </t>
   </si>
   <si>
-    <t>(1,808)</t>
+    <t>(1,813)</t>
   </si>
   <si>
     <t xml:space="preserve">Pushto
 </t>
   </si>
   <si>
-    <t>(1,639)</t>
+    <t>(1,643)</t>
   </si>
   <si>
     <t xml:space="preserve">Uzbek
 </t>
   </si>
   <si>
-    <t>(1,582)</t>
+    <t>(1,588)</t>
   </si>
   <si>
     <t xml:space="preserve">Azerbaijani
 </t>
   </si>
   <si>
-    <t>(1,350)</t>
+    <t>(1,353)</t>
   </si>
   <si>
     <t xml:space="preserve">Urdu
 </t>
   </si>
   <si>
-    <t>(1,335)</t>
+    <t>(1,338)</t>
   </si>
   <si>
     <t xml:space="preserve">Bengali
 </t>
   </si>
   <si>
-    <t>(1,329)</t>
+    <t>(1,332)</t>
   </si>
   <si>
     <t xml:space="preserve">Oriya
 </t>
   </si>
   <si>
-    <t>(260)</t>
+    <t>(261)</t>
   </si>
   <si>
     <t xml:space="preserve">Persian
@@ -265,7 +265,7 @@
 </t>
   </si>
   <si>
-    <t>(37)</t>
+    <t>(38)</t>
   </si>
   <si>
     <t xml:space="preserve">Hebrew

</xml_diff>